<commit_message>
fix bug, and finish gen ore veins
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -131,7 +131,7 @@
     <t>Surface Bismuthinite</t>
   </si>
   <si>
-    <t>Bismuth (90) (TFC)</t>
+    <t>Bismuth (90)</t>
   </si>
   <si>
     <t>Sulfur (3)</t>
@@ -467,7 +467,7 @@
     <t>Normal Redstone</t>
   </si>
   <si>
-    <t>Restone (45)</t>
+    <t>Redstone (45)</t>
   </si>
   <si>
     <t>Ruby (35)</t>
@@ -548,7 +548,7 @@
     <t>0.3</t>
   </si>
   <si>
-    <t>Shale, Claystone, Sylvite</t>
+    <t>Shale, Claystone</t>
   </si>
   <si>
     <t>Normal Beryllium</t>
@@ -656,7 +656,7 @@
     <t>Apatite (50)</t>
   </si>
   <si>
-    <t>TricalciumPhospate (35)</t>
+    <t>TricalciumPhosphate (35)</t>
   </si>
   <si>
     <t>Pyrochlore (15)</t>
@@ -689,7 +689,7 @@
     <t>GlauconiteSand (25)</t>
   </si>
   <si>
-    <t>Pentlandtite (15)</t>
+    <t>Pentlandite (15)</t>
   </si>
   <si>
     <t>Normal Mica</t>
@@ -755,7 +755,7 @@
     <t>Magnetite (5)</t>
   </si>
   <si>
-    <t>VanadiumMagnetiite (15)</t>
+    <t>VanadiumMagnetite (15)</t>
   </si>
   <si>
     <t>Chromite (60)</t>
@@ -782,10 +782,10 @@
     <t>Deep Garnet Amethyst</t>
   </si>
   <si>
-    <t>GarnetRed (5)</t>
-  </si>
-  <si>
-    <t>GarnetYellow (15)</t>
+    <t>RedGarnet (5)</t>
+  </si>
+  <si>
+    <t>YellowGarnet (15)</t>
   </si>
   <si>
     <t>Amethyst (65)</t>
@@ -821,7 +821,7 @@
     <t>Bornite (35)</t>
   </si>
   <si>
-    <t>Coopirite (25)</t>
+    <t>Cooperite (25)</t>
   </si>
   <si>
     <t>Platinum (25)</t>
@@ -860,7 +860,7 @@
     <t>Bornite (15)</t>
   </si>
   <si>
-    <t>Deep Molybdenium</t>
+    <t>Deep Molybdenum</t>
   </si>
   <si>
     <t>Wulfenite (40)</t>
@@ -869,7 +869,7 @@
     <t>Molybdenite (30)</t>
   </si>
   <si>
-    <t>Molybdenium (15)</t>
+    <t>Molybdenum (15)</t>
   </si>
   <si>
     <t>Powellite (15)</t>
@@ -881,7 +881,7 @@
     <t>Naquadah (75)</t>
   </si>
   <si>
-    <t>Plutonium239 (25)</t>
+    <t>Plutonium (25)</t>
   </si>
   <si>
     <t>Deep Pitchblende</t>

</xml_diff>